<commit_message>
1“ git commit -m1“
</commit_message>
<xml_diff>
--- a/duly.xlsx
+++ b/duly.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t>8月1日(周六)晚打球报名人员</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+  <si>
+    <t>8月8日(周六)晚打球报名人员</t>
   </si>
   <si>
     <t>姓名</t>
@@ -25,69 +25,81 @@
     <t>序号</t>
   </si>
   <si>
+    <t>邵祥毅</t>
+  </si>
+  <si>
+    <t>素白(1)</t>
+  </si>
+  <si>
+    <t>1(已收费)</t>
+  </si>
+  <si>
+    <t>程一航</t>
+  </si>
+  <si>
+    <t>Cheng</t>
+  </si>
+  <si>
     <t>小胖</t>
   </si>
   <si>
-    <t>1(已收费)</t>
-  </si>
-  <si>
-    <t>金理</t>
-  </si>
-  <si>
-    <t>2(已收费)</t>
+    <t>陈寿国</t>
+  </si>
+  <si>
+    <t>小c</t>
+  </si>
+  <si>
+    <t>蔡泽赟</t>
+  </si>
+  <si>
+    <t>陈昱嘉</t>
+  </si>
+  <si>
+    <t>素白(2)</t>
+  </si>
+  <si>
+    <t>4(已收费)</t>
+  </si>
+  <si>
+    <t>唐恺</t>
+  </si>
+  <si>
+    <t>官方提醒…注意</t>
   </si>
   <si>
     <t>阿正</t>
   </si>
   <si>
+    <t>朔</t>
+  </si>
+  <si>
     <t>Cocobolo(1)</t>
   </si>
   <si>
-    <t>4(已收费)</t>
+    <t>Cocobolo(2)</t>
+  </si>
+  <si>
+    <t>叶骏</t>
+  </si>
+  <si>
+    <t>暴躁的阿呆</t>
+  </si>
+  <si>
+    <t>韦恩</t>
   </si>
   <si>
     <t>黄镭</t>
   </si>
   <si>
-    <t>徐坤按门铃(2)</t>
-  </si>
-  <si>
-    <t>6(已收费)</t>
-  </si>
-  <si>
-    <t>Cocobolo(2)</t>
-  </si>
-  <si>
-    <t>7(已收费)</t>
-  </si>
-  <si>
-    <t>Cocobolo(3)</t>
-  </si>
-  <si>
-    <t>8(已收费)</t>
-  </si>
-  <si>
-    <t>枇杷</t>
-  </si>
-  <si>
-    <t>Cocobolo(4)</t>
-  </si>
-  <si>
-    <t>，1（标记）</t>
-  </si>
-  <si>
-    <t>11(已收费)</t>
-  </si>
-  <si>
-    <t>徐坤按门铃(1)</t>
-  </si>
-  <si>
-    <t>12(已收费)</t>
+    <t>王浩</t>
   </si>
   <si>
     <t>补位1</t>
   </si>
   <si>
+    <t>子远</t>
+  </si>
+  <si>
     <t>补位2</t>
   </si>
   <si>
@@ -97,16 +109,31 @@
     <t>补位4</t>
   </si>
   <si>
+    <t>朱枭鹏</t>
+  </si>
+  <si>
     <t>补位5</t>
   </si>
   <si>
+    <t>邵祥毅(1)</t>
+  </si>
+  <si>
     <t>补位6</t>
   </si>
   <si>
+    <t>邵祥毅(2)</t>
+  </si>
+  <si>
     <t>补位7</t>
   </si>
   <si>
+    <t>邵祥毅(3)</t>
+  </si>
+  <si>
     <t>补位8</t>
+  </si>
+  <si>
+    <t>Yb_3</t>
   </si>
   <si>
     <t>补位9</t>
@@ -129,10 +156,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -151,14 +178,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,6 +253,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -212,38 +269,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,38 +283,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,6 +342,138 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -327,13 +486,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,157 +504,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -527,8 +554,37 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -548,37 +604,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -598,26 +634,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -629,10 +656,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -641,137 +668,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -785,6 +812,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1109,15 +1139,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="2" width="16.7777777777778" customWidth="1"/>
+    <col min="6" max="6" width="17.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27" customHeight="1" spans="1:2">
@@ -1126,81 +1157,108 @@
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" ht="19" customHeight="1" spans="1:2">
+    <row r="2" ht="19" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" ht="19" customHeight="1" spans="1:2">
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" ht="19" customHeight="1" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" ht="19" customHeight="1" spans="1:2">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" ht="19" customHeight="1" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" ht="19" customHeight="1" spans="1:2">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" ht="19" customHeight="1" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" ht="19" customHeight="1" spans="1:2">
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="19" customHeight="1" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" ht="19" customHeight="1" spans="1:2">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="19" customHeight="1" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3">
         <v>5</v>
       </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" ht="19" customHeight="1" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6</v>
       </c>
     </row>
     <row r="9" ht="19" customHeight="1" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="B9" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="10" ht="19" customHeight="1" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8</v>
       </c>
     </row>
     <row r="11" ht="19" customHeight="1" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3">
         <v>9</v>
@@ -1208,7 +1266,7 @@
     </row>
     <row r="12" ht="19" customHeight="1" spans="1:2">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3">
         <v>10</v>
@@ -1216,96 +1274,114 @@
     </row>
     <row r="13" ht="19" customHeight="1" spans="1:2">
       <c r="A13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="B13" s="3">
+        <v>11</v>
       </c>
     </row>
     <row r="14" ht="19" customHeight="1" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="B14" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="15" ht="19" customHeight="1" spans="1:2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5" t="s">
-        <v>23</v>
+      <c r="A15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" ht="19" customHeight="1" spans="1:2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5" t="s">
-        <v>24</v>
+      <c r="A16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" ht="19" customHeight="1" spans="1:2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5" t="s">
-        <v>25</v>
+      <c r="A17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" ht="19" customHeight="1" spans="1:2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5" t="s">
-        <v>26</v>
+      <c r="A18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" ht="19" customHeight="1" spans="1:2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5" t="s">
-        <v>27</v>
+      <c r="A19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" ht="19" customHeight="1" spans="1:2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5" t="s">
-        <v>28</v>
+      <c r="A20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21" ht="19" customHeight="1" spans="1:2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5" t="s">
-        <v>29</v>
+      <c r="A21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="22" ht="19" customHeight="1" spans="1:2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5" t="s">
-        <v>30</v>
+      <c r="A22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" ht="19" customHeight="1" spans="1:2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5" t="s">
-        <v>31</v>
+      <c r="A23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24" ht="19" customHeight="1" spans="1:2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5" t="s">
-        <v>32</v>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="25" ht="19" customHeight="1" spans="1:2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5" t="s">
-        <v>33</v>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" ht="19" customHeight="1" spans="1:2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5" t="s">
-        <v>34</v>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" ht="19" customHeight="1" spans="1:2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5" t="s">
-        <v>35</v>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>